<commit_message>
Updated for Arabic Reports
</commit_message>
<xml_diff>
--- a/Powerbi_reports/PowerBi_keywords_Call 1-Call 3.xlsx
+++ b/Powerbi_reports/PowerBi_keywords_Call 1-Call 3.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -498,7 +498,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -528,7 +528,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -558,7 +558,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -588,7 +588,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -618,7 +618,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -648,7 +648,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -678,7 +678,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -738,7 +738,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -768,7 +768,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -824,7 +824,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -854,7 +854,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -884,7 +884,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -914,7 +914,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -944,7 +944,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -974,7 +974,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1004,7 +1004,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1034,7 +1034,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1064,7 +1064,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1094,7 +1094,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1124,7 +1124,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1154,7 +1154,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1184,7 +1184,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1214,7 +1214,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1244,7 +1244,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1274,7 +1274,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1304,7 +1304,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1360,7 +1360,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1390,7 +1390,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1450,7 +1450,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1480,7 +1480,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1510,7 +1510,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1570,7 +1570,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1600,7 +1600,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1630,7 +1630,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1660,7 +1660,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1690,7 +1690,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1720,7 +1720,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1750,7 +1750,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Call 1.wav</t>
+          <t>Call 1</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1780,7 +1780,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1810,7 +1810,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1870,7 +1870,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1900,7 +1900,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1930,7 +1930,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1960,7 +1960,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1990,7 +1990,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2020,7 +2020,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2050,7 +2050,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2080,7 +2080,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2110,7 +2110,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2218,7 +2218,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2248,7 +2248,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2278,7 +2278,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2334,7 +2334,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2364,7 +2364,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2394,7 +2394,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2450,7 +2450,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2480,7 +2480,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2510,7 +2510,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2540,7 +2540,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2570,7 +2570,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2600,7 +2600,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2630,7 +2630,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2660,7 +2660,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2690,7 +2690,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2746,7 +2746,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2776,7 +2776,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2806,7 +2806,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2836,7 +2836,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2866,7 +2866,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2896,7 +2896,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Call 2.wav</t>
+          <t>Call 2</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2926,7 +2926,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2956,7 +2956,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2986,7 +2986,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3016,7 +3016,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3046,7 +3046,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3076,7 +3076,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3106,7 +3106,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3136,7 +3136,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3166,7 +3166,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3196,7 +3196,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3226,7 +3226,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3256,7 +3256,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3316,7 +3316,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3346,7 +3346,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3376,7 +3376,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3406,7 +3406,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3436,7 +3436,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3466,7 +3466,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3496,7 +3496,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3526,7 +3526,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3556,7 +3556,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -3586,7 +3586,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3616,7 +3616,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3646,7 +3646,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3676,7 +3676,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3732,7 +3732,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3762,7 +3762,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3792,7 +3792,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3822,7 +3822,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3852,7 +3852,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Call 3.wav</t>
+          <t>Call 3</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">

</xml_diff>